<commit_message>
1.1 add filter and sort
</commit_message>
<xml_diff>
--- a/komputronik.xlsx
+++ b/komputronik.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,73 +424,361 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>PNY GeForce RTX 3060 12GB XLR8 Gaming REVEL EPIC-X RGB Single Fan</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>1779</t>
-        </is>
+          <t>Gigabyte GeForce RTX 3060 EAGLE 12GB OC 2.0 LHR</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1519</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Palit GeForce RTX 3060 StormX</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3699</t>
-        </is>
+          <t>Gigabyte GeForce RTX 3060 Gaming 12GB OC 2.0 LHR</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1499</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PNY GeForce RTX 3060 12GB Uprising Dual Fan</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4749</t>
-        </is>
+          <t>ASUS GeForce RTX 3060 DUAL 12GB OC V2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1629</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PNY GeForce RTX 3060 VERTO 8GB Dual Fan Edition</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1459</t>
-        </is>
+          <t>ASUS GeForce RTX 3060 TUF 12GB OC V2 LHR</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1829</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Inno3D GeForce RTX 3060 Twin X2 8GB GDDR6</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1679</t>
-        </is>
+          <t>ASUS GeForce RTX 3060 DUAL 8GB OC WHITE</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1429</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Gigabyte GeForce RTX 3060 WindForce 12GB OC</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ASUS GeForce RTX 3060 DUAL 8GB OC</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gigabyte GeForce RTX 3060 VISION 12GB OC 2.0 LHR</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MSI GeForce RTX 3060 VENTUS 2X 12GB OC LHR</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gainward GeForce RTX 3060 Ghost 12GB</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ASUS GeForce RTX 3060 PHOENIX 12GB V2 LHR</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ZOTAC Gaming GeForce RTX 3060 Twin Edge OC 12GB</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Inno3D GeForce RTX 3060 Twin X2 LHR 12GB GDDR6</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Gigabyte GeForce RTX 3060 Gaming 8GB OC</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Palit GeForce RTX 3060 Dual 12GB</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ZOTAC Gaming GeForce RTX 3060 Twin Edge 12GB</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Palit GeForce RTX 3060 Dual 12GB OC</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Inno3D GeForce RTX 3060 Twin X2 OC 8GB GDDR6</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MSI GeForce RTX 3060 GAMING X 12GB LHR</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MSI GeForce RTX 3060 VENTUS 3X 12GB OC LHR</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MSI GeForce RTX 3060 VENTUS 2X 8GB OC LHR</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>MSI GeForce RTX 3060 AERO ITX 12GB OC LHR</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ZOTAC Gaming GeForce RTX 3060 AMP White Edition 12GB</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Inno3D GeForce RTX 3060 Twin X2 OC LHR 12GB GDDR6</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Gainward GeForce RTX 3060 Ghost 12GB OC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Gigabyte GeForce RTX 3060 AORUS ELITE 12GB 2.0 LHR</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Gainward GeForce RTX 3060 Pegasus OC 12GB</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3699</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Gainward GeForce RTX 3060 Pegasus 12GB</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ZOTAC Gaming GeForce RTX 3060 Twin Edge 8GB</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>MSI GeForce RTX 3060 GAMING Z 12GB LHR</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>PNY GeForce RTX 3060 12GB XLR8 Gaming REVEL EPIC-X RGB Single Fan</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Palit GeForce RTX 3060 StormX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3699</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PNY GeForce RTX 3060 12GB Uprising Dual Fan</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PNY GeForce RTX 3060 VERTO 8GB Dual Fan Edition</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Inno3D GeForce RTX 3060 Twin X2 8GB GDDR6</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>PNY GeForce RTX 3060 12GB XLR8 Gaming REVEL EPIC-X RGB Dual Fan</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2049</t>
-        </is>
+      <c r="B36" t="n">
+        <v>2049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>